<commit_message>
Actualizacion Métricas y Diagrama de Clases.
</commit_message>
<xml_diff>
--- a/Documentacion/MatrizMath/MatrizMath - Planilla de Métricas V2.1.xlsx.xlsx
+++ b/Documentacion/MatrizMath/MatrizMath - Planilla de Métricas V2.1.xlsx.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900"/>
   </bookViews>
   <sheets>
     <sheet name="Métricas" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
   <si>
     <t>PROYECTO:</t>
   </si>
@@ -137,6 +137,24 @@
   <si>
     <t>atributos, constructores getters y setters</t>
   </si>
+  <si>
+    <t>productoDeUnaFila()</t>
+  </si>
+  <si>
+    <t>intercambiarFilas()</t>
+  </si>
+  <si>
+    <t>sumarFilas()</t>
+  </si>
+  <si>
+    <t>intercambiarConRenglonNoNuloPorDebajo()</t>
+  </si>
+  <si>
+    <t>intercambiarConRenglonNoNuloPorArriba()</t>
+  </si>
+  <si>
+    <t>llevarACeroPosicionesPorDebajo()</t>
+  </si>
 </sst>
 </file>
 
@@ -146,7 +164,7 @@
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -184,6 +202,25 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -744,7 +781,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -956,53 +993,41 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1014,24 +1039,458 @@
     <xf numFmtId="1" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="7" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="7" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="7" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFFFFFF"/>
@@ -1186,7 +1645,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Métricas!$B$37:$B$42</c:f>
+              <c:f>Métricas!$B$43:$B$48</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1212,7 +1671,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Métricas!$C$37:$C$42</c:f>
+              <c:f>Métricas!$C$43:$C$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1265,13 +1724,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1557,17 +2016,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="11" width="10" customWidth="1"/>
+    <col min="3" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="6" max="11" width="10" customWidth="1"/>
     <col min="12" max="12" width="11.42578125" customWidth="1"/>
     <col min="13" max="14" width="10" customWidth="1"/>
     <col min="15" max="15" width="1" customWidth="1"/>
@@ -1577,23 +2038,23 @@
   <sheetData>
     <row r="1" spans="1:26" ht="23.25" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="103" t="s">
+      <c r="B1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="102" t="s">
+      <c r="C1" s="73"/>
+      <c r="D1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="100"/>
-      <c r="L1" s="100"/>
-      <c r="M1" s="100"/>
-      <c r="N1" s="100"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -1637,12 +2098,12 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
       <c r="A3" s="4"/>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="84"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="76"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -1768,12 +2229,12 @@
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" s="4"/>
-      <c r="B7" s="82" t="s">
+      <c r="B7" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="83"/>
-      <c r="D7" s="83"/>
-      <c r="E7" s="84"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="76"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -1810,15 +2271,15 @@
       <c r="E8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="99"/>
-      <c r="G8" s="100"/>
-      <c r="H8" s="100"/>
-      <c r="I8" s="100"/>
-      <c r="J8" s="100"/>
-      <c r="K8" s="100"/>
-      <c r="L8" s="100"/>
-      <c r="M8" s="100"/>
-      <c r="N8" s="100"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
+      <c r="M8" s="73"/>
+      <c r="N8" s="73"/>
       <c r="O8" s="7"/>
       <c r="P8" s="13"/>
       <c r="Q8" s="14"/>
@@ -1845,15 +2306,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C9),ISBLANK(D9)),"Completar",IF(D9&gt;=C9,D9-C9,"Error")),"Error")</f>
         <v>Completar</v>
       </c>
-      <c r="F9" s="101"/>
-      <c r="G9" s="100"/>
-      <c r="H9" s="100"/>
-      <c r="I9" s="100"/>
-      <c r="J9" s="100"/>
-      <c r="K9" s="100"/>
-      <c r="L9" s="100"/>
-      <c r="M9" s="100"/>
-      <c r="N9" s="100"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="73"/>
+      <c r="N9" s="73"/>
       <c r="O9" s="15"/>
       <c r="P9" s="21"/>
       <c r="Q9" s="22"/>
@@ -1897,12 +2358,12 @@
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" s="4"/>
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="83"/>
-      <c r="D11" s="83"/>
-      <c r="E11" s="84"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="76"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -1939,15 +2400,15 @@
       <c r="E12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="99"/>
-      <c r="G12" s="100"/>
-      <c r="H12" s="100"/>
-      <c r="I12" s="100"/>
-      <c r="J12" s="100"/>
-      <c r="K12" s="100"/>
-      <c r="L12" s="100"/>
-      <c r="M12" s="100"/>
-      <c r="N12" s="100"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="73"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="73"/>
+      <c r="L12" s="73"/>
+      <c r="M12" s="73"/>
+      <c r="N12" s="73"/>
       <c r="O12" s="7"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="14"/>
@@ -1972,15 +2433,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C13),ISBLANK(D13)),"Completar",IF(D13&gt;=C13,D13-C13,"Error")),"Error")</f>
         <v>Completar</v>
       </c>
-      <c r="F13" s="101"/>
-      <c r="G13" s="100"/>
-      <c r="H13" s="100"/>
-      <c r="I13" s="100"/>
-      <c r="J13" s="100"/>
-      <c r="K13" s="100"/>
-      <c r="L13" s="100"/>
-      <c r="M13" s="100"/>
-      <c r="N13" s="100"/>
+      <c r="F13" s="79"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="73"/>
+      <c r="L13" s="73"/>
+      <c r="M13" s="73"/>
+      <c r="N13" s="73"/>
       <c r="O13" s="15"/>
       <c r="P13" s="21"/>
       <c r="Q13" s="22"/>
@@ -2024,21 +2485,21 @@
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
       <c r="A15" s="4"/>
-      <c r="B15" s="82" t="s">
+      <c r="B15" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="83"/>
-      <c r="D15" s="83"/>
-      <c r="E15" s="83"/>
-      <c r="F15" s="83"/>
-      <c r="G15" s="83"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="83"/>
-      <c r="J15" s="83"/>
-      <c r="K15" s="83"/>
-      <c r="L15" s="83"/>
-      <c r="M15" s="83"/>
-      <c r="N15" s="84"/>
+      <c r="C15" s="75"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="75"/>
+      <c r="I15" s="75"/>
+      <c r="J15" s="75"/>
+      <c r="K15" s="75"/>
+      <c r="L15" s="75"/>
+      <c r="M15" s="75"/>
+      <c r="N15" s="76"/>
       <c r="O15" s="4"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
@@ -2054,31 +2515,31 @@
     </row>
     <row r="16" spans="1:26" ht="16.5" customHeight="1">
       <c r="A16" s="7"/>
-      <c r="B16" s="73" t="s">
+      <c r="B16" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="75" t="s">
+      <c r="C16" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="76"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="71" t="s">
+      <c r="D16" s="102"/>
+      <c r="E16" s="102"/>
+      <c r="F16" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="72"/>
-      <c r="H16" s="81" t="s">
+      <c r="G16" s="95"/>
+      <c r="H16" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="80"/>
-      <c r="J16" s="80"/>
-      <c r="K16" s="71" t="s">
+      <c r="I16" s="81"/>
+      <c r="J16" s="81"/>
+      <c r="K16" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="L16" s="72"/>
-      <c r="M16" s="87" t="s">
+      <c r="L16" s="95"/>
+      <c r="M16" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="N16" s="89" t="s">
+      <c r="N16" s="91" t="s">
         <v>6</v>
       </c>
       <c r="O16" s="7"/>
@@ -2096,10 +2557,10 @@
     </row>
     <row r="17" spans="1:26" ht="30" customHeight="1">
       <c r="A17" s="7"/>
-      <c r="B17" s="74"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
+      <c r="B17" s="100"/>
+      <c r="C17" s="103"/>
+      <c r="D17" s="104"/>
+      <c r="E17" s="104"/>
       <c r="F17" s="26" t="s">
         <v>16</v>
       </c>
@@ -2121,8 +2582,8 @@
       <c r="L17" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="M17" s="88"/>
-      <c r="N17" s="90"/>
+      <c r="M17" s="98"/>
+      <c r="N17" s="92"/>
       <c r="O17" s="7"/>
       <c r="P17" s="13"/>
       <c r="Q17" s="14"/>
@@ -2139,14 +2600,14 @@
     <row r="18" spans="1:26">
       <c r="A18" s="15"/>
       <c r="B18" s="30">
-        <f t="shared" ref="B18:B25" si="0">ROW($B18)-16</f>
+        <f t="shared" ref="B18:B31" si="0">ROW($B18)-16</f>
         <v>2</v>
       </c>
-      <c r="C18" s="79" t="s">
+      <c r="C18" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="80"/>
-      <c r="E18" s="80"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="81"/>
       <c r="F18" s="31">
         <v>60</v>
       </c>
@@ -2160,7 +2621,7 @@
         <v>0.68819444444444444</v>
       </c>
       <c r="J18" s="35">
-        <f t="shared" ref="J18:J23" si="1">IFERROR(IF(OR(ISBLANK(H18),ISBLANK(I18)),"",IF(I18&gt;=H18,I18-H18,"Error")),"Error")</f>
+        <f t="shared" ref="J18:J31" si="1">IFERROR(IF(OR(ISBLANK(H18),ISBLANK(I18)),"",IF(I18&gt;=H18,I18-H18,"Error")),"Error")</f>
         <v>2.1527777777777812E-2</v>
       </c>
       <c r="K18" s="36">
@@ -2173,7 +2634,7 @@
         <v>55</v>
       </c>
       <c r="N18" s="39">
-        <f t="shared" ref="N18:N23" si="2">IFERROR(IF(OR(J18="",ISBLANK(L18)),"",J18+L18),"Error")</f>
+        <f t="shared" ref="N18:N31" si="2">IFERROR(IF(OR(J18="",ISBLANK(L18)),"",J18+L18),"Error")</f>
         <v>2.9166666666666702E-2</v>
       </c>
       <c r="O18" s="15"/>
@@ -2195,11 +2656,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C19" s="79" t="s">
+      <c r="C19" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="80"/>
-      <c r="E19" s="80"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
       <c r="F19" s="31">
         <v>4</v>
       </c>
@@ -2248,11 +2709,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C20" s="79" t="s">
+      <c r="C20" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="80"/>
-      <c r="E20" s="80"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="81"/>
       <c r="F20" s="31">
         <v>8</v>
       </c>
@@ -2301,11 +2762,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C21" s="79" t="s">
+      <c r="C21" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="80"/>
-      <c r="E21" s="80"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
       <c r="F21" s="31">
         <v>10</v>
       </c>
@@ -2348,42 +2809,58 @@
       <c r="Y21" s="22"/>
       <c r="Z21" s="22"/>
     </row>
-    <row r="22" spans="1:26">
-      <c r="A22" s="15"/>
-      <c r="B22" s="30">
+    <row r="22" spans="1:26" s="121" customFormat="1">
+      <c r="A22" s="106"/>
+      <c r="B22" s="107">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C22" s="79"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="35" t="str">
+      <c r="C22" s="108" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="109"/>
+      <c r="E22" s="109"/>
+      <c r="F22" s="110">
+        <v>8</v>
+      </c>
+      <c r="G22" s="111">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="H22" s="112">
+        <v>0.6777777777777777</v>
+      </c>
+      <c r="I22" s="113">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="J22" s="114">
         <f t="shared" si="1"/>
-        <v/>
+        <v>1.3194444444444509E-2</v>
       </c>
-      <c r="K22" s="46"/>
-      <c r="L22" s="47"/>
-      <c r="M22" s="48"/>
-      <c r="N22" s="39" t="str">
+      <c r="K22" s="115">
+        <v>1</v>
+      </c>
+      <c r="L22" s="116">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="M22" s="117">
+        <v>12</v>
+      </c>
+      <c r="N22" s="118">
         <f t="shared" si="2"/>
-        <v/>
+        <v>1.6666666666666732E-2</v>
       </c>
-      <c r="O22" s="15"/>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="22"/>
-      <c r="S22" s="22"/>
-      <c r="T22" s="22"/>
-      <c r="U22" s="22"/>
-      <c r="V22" s="22"/>
-      <c r="W22" s="22"/>
-      <c r="X22" s="22"/>
-      <c r="Y22" s="22"/>
-      <c r="Z22" s="22"/>
+      <c r="O22" s="106"/>
+      <c r="P22" s="119"/>
+      <c r="Q22" s="120"/>
+      <c r="R22" s="120"/>
+      <c r="S22" s="120"/>
+      <c r="T22" s="120"/>
+      <c r="U22" s="120"/>
+      <c r="V22" s="120"/>
+      <c r="W22" s="120"/>
+      <c r="X22" s="120"/>
+      <c r="Y22" s="120"/>
+      <c r="Z22" s="120"/>
     </row>
     <row r="23" spans="1:26">
       <c r="A23" s="15"/>
@@ -2391,23 +2868,39 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C23" s="79"/>
-      <c r="D23" s="80"/>
-      <c r="E23" s="80"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="35" t="str">
+      <c r="C23" s="105" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="81"/>
+      <c r="E23" s="81"/>
+      <c r="F23" s="42">
+        <v>13</v>
+      </c>
+      <c r="G23" s="43">
+        <v>1.2499999999999999E-2</v>
+      </c>
+      <c r="H23" s="44">
+        <v>0.6958333333333333</v>
+      </c>
+      <c r="I23" s="45">
+        <v>0.7055555555555556</v>
+      </c>
+      <c r="J23" s="35">
         <f t="shared" si="1"/>
-        <v/>
+        <v>9.7222222222222987E-3</v>
       </c>
-      <c r="K23" s="46"/>
-      <c r="L23" s="47"/>
-      <c r="M23" s="48"/>
-      <c r="N23" s="39" t="str">
+      <c r="K23" s="46">
+        <v>0</v>
+      </c>
+      <c r="L23" s="47">
+        <v>0</v>
+      </c>
+      <c r="M23" s="48">
+        <v>16</v>
+      </c>
+      <c r="N23" s="39">
         <f t="shared" si="2"/>
-        <v/>
+        <v>9.7222222222222987E-3</v>
       </c>
       <c r="O23" s="15"/>
       <c r="P23" s="21"/>
@@ -2428,18 +2921,40 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C24" s="79"/>
-      <c r="D24" s="80"/>
-      <c r="E24" s="80"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="46"/>
-      <c r="L24" s="47"/>
-      <c r="M24" s="48"/>
-      <c r="N24" s="39"/>
+      <c r="C24" s="105" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="42">
+        <v>25</v>
+      </c>
+      <c r="G24" s="43">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="H24" s="44">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="I24" s="45">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="J24" s="35">
+        <f t="shared" si="1"/>
+        <v>9.7222222222221877E-3</v>
+      </c>
+      <c r="K24" s="46">
+        <v>2</v>
+      </c>
+      <c r="L24" s="47">
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="M24" s="48">
+        <v>13</v>
+      </c>
+      <c r="N24" s="39">
+        <f t="shared" si="2"/>
+        <v>1.5277777777777744E-2</v>
+      </c>
       <c r="O24" s="15"/>
       <c r="P24" s="21"/>
       <c r="Q24" s="22"/>
@@ -2454,30 +2969,46 @@
       <c r="Z24" s="22"/>
     </row>
     <row r="25" spans="1:26">
-      <c r="A25" s="15"/>
+      <c r="A25" s="71"/>
       <c r="B25" s="30">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C25" s="79"/>
-      <c r="D25" s="80"/>
-      <c r="E25" s="80"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="35" t="str">
-        <f>IFERROR(IF(OR(ISBLANK(H25),ISBLANK(I25)),"",IF(I25&gt;=H25,I25-H25,"Error")),"Error")</f>
-        <v/>
+      <c r="C25" s="105" t="s">
+        <v>43</v>
       </c>
-      <c r="K25" s="46"/>
-      <c r="L25" s="47"/>
-      <c r="M25" s="48"/>
-      <c r="N25" s="39" t="str">
-        <f>IFERROR(IF(OR(J25="",ISBLANK(L25)),"",J25+L25),"Error")</f>
-        <v/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="81"/>
+      <c r="F25" s="42">
+        <v>20</v>
       </c>
-      <c r="O25" s="15"/>
+      <c r="G25" s="43">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="H25" s="44">
+        <v>0.7368055555555556</v>
+      </c>
+      <c r="I25" s="45">
+        <v>0.74930555555555556</v>
+      </c>
+      <c r="J25" s="35">
+        <f t="shared" si="1"/>
+        <v>1.2499999999999956E-2</v>
+      </c>
+      <c r="K25" s="46">
+        <v>0</v>
+      </c>
+      <c r="L25" s="47">
+        <v>0</v>
+      </c>
+      <c r="M25" s="48">
+        <v>16</v>
+      </c>
+      <c r="N25" s="39">
+        <f t="shared" si="2"/>
+        <v>1.2499999999999956E-2</v>
+      </c>
+      <c r="O25" s="71"/>
       <c r="P25" s="21"/>
       <c r="Q25" s="22"/>
       <c r="R25" s="22"/>
@@ -2490,174 +3021,211 @@
       <c r="Y25" s="22"/>
       <c r="Z25" s="22"/>
     </row>
-    <row r="26" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A26" s="7"/>
-      <c r="B26" s="85" t="s">
-        <v>23</v>
+    <row r="26" spans="1:26" ht="15" customHeight="1">
+      <c r="A26" s="71"/>
+      <c r="B26" s="30">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
-      <c r="C26" s="86"/>
-      <c r="D26" s="86"/>
-      <c r="E26" s="86"/>
-      <c r="F26" s="49">
-        <f t="shared" ref="F26:G26" si="3">IF(SUM(F18:F25)=0,"Completar",SUM(F18:F25))</f>
-        <v>82</v>
+      <c r="C26" s="105" t="s">
+        <v>42</v>
       </c>
-      <c r="G26" s="50">
-        <f t="shared" si="3"/>
-        <v>3.4722222222222224E-2</v>
+      <c r="D26" s="81"/>
+      <c r="E26" s="81"/>
+      <c r="F26" s="42">
+        <v>16</v>
       </c>
-      <c r="H26" s="51" t="s">
-        <v>24</v>
+      <c r="G26" s="43">
+        <v>1.3888888888888888E-2</v>
       </c>
-      <c r="I26" s="52" t="s">
-        <v>24</v>
+      <c r="H26" s="44">
+        <v>0.75069444444444444</v>
       </c>
-      <c r="J26" s="53">
-        <f>IF(OR(COUNTIF(J18:J25,"Error")&gt;0,COUNTIF(J18:J25,"Completar")&gt;0),"Error",IF(SUM(J18:J25)=0,"Completar",SUM(J18:J25)))</f>
-        <v>3.472222222222221E-2</v>
+      <c r="I26" s="45">
+        <v>0.75694444444444453</v>
       </c>
-      <c r="K26" s="54">
-        <f t="shared" ref="K26:L26" si="4">SUM(K18:K25)</f>
-        <v>4</v>
+      <c r="J26" s="35">
+        <f t="shared" si="1"/>
+        <v>6.2500000000000888E-3</v>
       </c>
-      <c r="L26" s="50">
-        <f t="shared" si="4"/>
-        <v>7.6388888888888886E-3</v>
+      <c r="K26" s="46">
+        <v>1</v>
       </c>
-      <c r="M26" s="55">
-        <f>IF(SUM(M18:M25)=0,"Completar",SUM(M18:M25))</f>
-        <v>85</v>
+      <c r="L26" s="47">
+        <v>6.9444444444444447E-4</v>
       </c>
-      <c r="N26" s="18">
-        <f>IF(OR(COUNTIF(N18:N25,"Error")&gt;0,COUNTIF(N18:N25,"Completar")&gt;0),"Error",IF(SUM(N18:N25)=0,"Completar",SUM(N18:N25)))</f>
-        <v>4.2361111111111099E-2</v>
+      <c r="M26" s="48">
+        <v>16</v>
       </c>
-      <c r="O26" s="7"/>
-      <c r="P26" s="56"/>
-      <c r="Q26" s="57"/>
-      <c r="R26" s="57"/>
-      <c r="S26" s="57"/>
-      <c r="T26" s="57"/>
-      <c r="U26" s="57"/>
-      <c r="V26" s="57"/>
-      <c r="W26" s="57"/>
-      <c r="X26" s="57"/>
-      <c r="Y26" s="57"/>
-      <c r="Z26" s="57"/>
-    </row>
-    <row r="27" spans="1:26" ht="6" customHeight="1">
-      <c r="A27" s="20"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20"/>
-      <c r="O27" s="20"/>
-      <c r="P27" s="23"/>
-      <c r="Q27" s="23"/>
-      <c r="R27" s="23"/>
-      <c r="S27" s="23"/>
-      <c r="T27" s="23"/>
-      <c r="U27" s="23"/>
-      <c r="V27" s="23"/>
-      <c r="W27" s="23"/>
-      <c r="X27" s="23"/>
-      <c r="Y27" s="23"/>
-      <c r="Z27" s="23"/>
+      <c r="N26" s="39">
+        <f t="shared" si="2"/>
+        <v>6.9444444444445334E-3</v>
+      </c>
+      <c r="O26" s="71"/>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="22"/>
+      <c r="S26" s="22"/>
+      <c r="T26" s="22"/>
+      <c r="U26" s="22"/>
+      <c r="V26" s="22"/>
+      <c r="W26" s="22"/>
+      <c r="X26" s="22"/>
+      <c r="Y26" s="22"/>
+      <c r="Z26" s="22"/>
+    </row>
+    <row r="27" spans="1:26" ht="15" customHeight="1">
+      <c r="A27" s="71"/>
+      <c r="B27" s="30">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C27" s="105" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="42">
+        <v>30</v>
+      </c>
+      <c r="G27" s="43">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="H27" s="44">
+        <v>0.75902777777777775</v>
+      </c>
+      <c r="I27" s="45">
+        <v>0.77430555555555547</v>
+      </c>
+      <c r="J27" s="35">
+        <f t="shared" si="1"/>
+        <v>1.5277777777777724E-2</v>
+      </c>
+      <c r="K27" s="46">
+        <v>0</v>
+      </c>
+      <c r="L27" s="47">
+        <v>0</v>
+      </c>
+      <c r="M27" s="48">
+        <v>17</v>
+      </c>
+      <c r="N27" s="39">
+        <f t="shared" si="2"/>
+        <v>1.5277777777777724E-2</v>
+      </c>
+      <c r="O27" s="71"/>
+      <c r="P27" s="21"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="22"/>
+      <c r="U27" s="22"/>
+      <c r="V27" s="22"/>
+      <c r="W27" s="22"/>
+      <c r="X27" s="22"/>
+      <c r="Y27" s="22"/>
+      <c r="Z27" s="22"/>
     </row>
     <row r="28" spans="1:26" ht="15" customHeight="1">
-      <c r="A28" s="4"/>
-      <c r="B28" s="82" t="s">
-        <v>25</v>
+      <c r="A28" s="71"/>
+      <c r="B28" s="30">
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
-      <c r="C28" s="83"/>
-      <c r="D28" s="83"/>
-      <c r="E28" s="84"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="6"/>
-      <c r="R28" s="6"/>
-      <c r="S28" s="6"/>
-      <c r="T28" s="6"/>
-      <c r="U28" s="6"/>
-      <c r="V28" s="6"/>
-      <c r="W28" s="6"/>
-      <c r="X28" s="6"/>
-      <c r="Y28" s="6"/>
-      <c r="Z28" s="6"/>
-    </row>
-    <row r="29" spans="1:26" ht="30" customHeight="1">
-      <c r="A29" s="7"/>
-      <c r="B29" s="8" t="s">
-        <v>3</v>
+      <c r="C28" s="105"/>
+      <c r="D28" s="81"/>
+      <c r="E28" s="81"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>4</v>
+      <c r="K28" s="46"/>
+      <c r="L28" s="47"/>
+      <c r="M28" s="48"/>
+      <c r="N28" s="39" t="str">
+        <f t="shared" si="2"/>
+        <v/>
       </c>
-      <c r="D29" s="9" t="s">
-        <v>5</v>
+      <c r="O28" s="71"/>
+      <c r="P28" s="21"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22"/>
+      <c r="U28" s="22"/>
+      <c r="V28" s="22"/>
+      <c r="W28" s="22"/>
+      <c r="X28" s="22"/>
+      <c r="Y28" s="22"/>
+      <c r="Z28" s="22"/>
+    </row>
+    <row r="29" spans="1:26" ht="15" customHeight="1">
+      <c r="A29" s="71"/>
+      <c r="B29" s="30">
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
-      <c r="E29" s="10" t="s">
-        <v>6</v>
+      <c r="C29" s="105"/>
+      <c r="D29" s="81"/>
+      <c r="E29" s="81"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
-      <c r="P29" s="13"/>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="14"/>
-      <c r="S29" s="14"/>
-      <c r="T29" s="14"/>
-      <c r="U29" s="14"/>
-      <c r="V29" s="14"/>
-      <c r="W29" s="14"/>
-      <c r="X29" s="14"/>
-      <c r="Y29" s="14"/>
-      <c r="Z29" s="14"/>
-    </row>
-    <row r="30" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A30" s="15"/>
-      <c r="B30" s="58"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="18" t="str">
-        <f>IFERROR(IF(OR(ISBLANK(C30),ISBLANK(D30)),"Completar",IF(D30&gt;=C30,D30-C30,"Error")),"Error")</f>
-        <v>Completar</v>
+      <c r="K29" s="46"/>
+      <c r="L29" s="47"/>
+      <c r="M29" s="48"/>
+      <c r="N29" s="39" t="str">
+        <f t="shared" si="2"/>
+        <v/>
       </c>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
+      <c r="O29" s="71"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="22"/>
+      <c r="S29" s="22"/>
+      <c r="T29" s="22"/>
+      <c r="U29" s="22"/>
+      <c r="V29" s="22"/>
+      <c r="W29" s="22"/>
+      <c r="X29" s="22"/>
+      <c r="Y29" s="22"/>
+      <c r="Z29" s="22"/>
+    </row>
+    <row r="30" spans="1:26" ht="15" customHeight="1">
+      <c r="A30" s="71"/>
+      <c r="B30" s="30">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C30" s="105"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="81"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K30" s="46"/>
+      <c r="L30" s="47"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="39" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O30" s="71"/>
       <c r="P30" s="21"/>
       <c r="Q30" s="22"/>
       <c r="R30" s="22"/>
@@ -2670,255 +3238,268 @@
       <c r="Y30" s="22"/>
       <c r="Z30" s="22"/>
     </row>
-    <row r="31" spans="1:26" ht="6" customHeight="1">
-      <c r="A31" s="20"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="20"/>
-      <c r="O31" s="20"/>
-      <c r="P31" s="23"/>
-      <c r="Q31" s="23"/>
-      <c r="R31" s="23"/>
-      <c r="S31" s="23"/>
-      <c r="T31" s="23"/>
-      <c r="U31" s="23"/>
-      <c r="V31" s="23"/>
-      <c r="W31" s="23"/>
-      <c r="X31" s="23"/>
-      <c r="Y31" s="23"/>
-      <c r="Z31" s="23"/>
-    </row>
-    <row r="32" spans="1:26">
-      <c r="A32" s="20"/>
-      <c r="B32" s="82" t="s">
+    <row r="31" spans="1:26">
+      <c r="A31" s="71"/>
+      <c r="B31" s="30">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C31" s="105"/>
+      <c r="D31" s="81"/>
+      <c r="E31" s="81"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="44"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K31" s="46"/>
+      <c r="L31" s="47"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="39" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O31" s="71"/>
+      <c r="P31" s="21"/>
+      <c r="Q31" s="22"/>
+      <c r="R31" s="22"/>
+      <c r="S31" s="22"/>
+      <c r="T31" s="22"/>
+      <c r="U31" s="22"/>
+      <c r="V31" s="22"/>
+      <c r="W31" s="22"/>
+      <c r="X31" s="22"/>
+      <c r="Y31" s="22"/>
+      <c r="Z31" s="22"/>
+    </row>
+    <row r="32" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A32" s="7"/>
+      <c r="B32" s="96" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="86"/>
+      <c r="D32" s="86"/>
+      <c r="E32" s="86"/>
+      <c r="F32" s="49">
+        <f>IF(SUM(F18:F31)=0,"Completar",SUM(F18:F31))</f>
+        <v>194</v>
+      </c>
+      <c r="G32" s="50">
+        <f>IF(SUM(G18:G31)=0,"Completar",SUM(G18:G31))</f>
+        <v>0.12361111111111112</v>
+      </c>
+      <c r="H32" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I32" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="J32" s="53">
+        <f>IF(OR(COUNTIF(J18:J31,"Error")&gt;0,COUNTIF(J18:J31,"Completar")&gt;0),"Error",IF(SUM(J18:J31)=0,"Completar",SUM(J18:J31)))</f>
+        <v>0.10138888888888897</v>
+      </c>
+      <c r="K32" s="54">
+        <f>SUM(K18:K31)</f>
+        <v>8</v>
+      </c>
+      <c r="L32" s="50">
+        <f>SUM(L18:L31)</f>
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="M32" s="55">
+        <f>IF(SUM(M18:M31)=0,"Completar",SUM(M18:M31))</f>
+        <v>175</v>
+      </c>
+      <c r="N32" s="18">
+        <f>IF(OR(COUNTIF(N18:N31,"Error")&gt;0,COUNTIF(N18:N31,"Completar")&gt;0),"Error",IF(SUM(N18:N31)=0,"Completar",SUM(N18:N31)))</f>
+        <v>0.11875000000000008</v>
+      </c>
+      <c r="O32" s="7"/>
+      <c r="P32" s="56"/>
+      <c r="Q32" s="57"/>
+      <c r="R32" s="57"/>
+      <c r="S32" s="57"/>
+      <c r="T32" s="57"/>
+      <c r="U32" s="57"/>
+      <c r="V32" s="57"/>
+      <c r="W32" s="57"/>
+      <c r="X32" s="57"/>
+      <c r="Y32" s="57"/>
+      <c r="Z32" s="57"/>
+    </row>
+    <row r="33" spans="1:26" ht="6" customHeight="1">
+      <c r="A33" s="20"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="20"/>
+      <c r="O33" s="20"/>
+      <c r="P33" s="23"/>
+      <c r="Q33" s="23"/>
+      <c r="R33" s="23"/>
+      <c r="S33" s="23"/>
+      <c r="T33" s="23"/>
+      <c r="U33" s="23"/>
+      <c r="V33" s="23"/>
+      <c r="W33" s="23"/>
+      <c r="X33" s="23"/>
+      <c r="Y33" s="23"/>
+      <c r="Z33" s="23"/>
+    </row>
+    <row r="34" spans="1:26" ht="15" customHeight="1">
+      <c r="A34" s="4"/>
+      <c r="B34" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="75"/>
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="6"/>
+      <c r="S34" s="6"/>
+      <c r="T34" s="6"/>
+      <c r="U34" s="6"/>
+      <c r="V34" s="6"/>
+      <c r="W34" s="6"/>
+      <c r="X34" s="6"/>
+      <c r="Y34" s="6"/>
+      <c r="Z34" s="6"/>
+    </row>
+    <row r="35" spans="1:26" ht="30" customHeight="1">
+      <c r="A35" s="7"/>
+      <c r="B35" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="13"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="14"/>
+      <c r="S35" s="14"/>
+      <c r="T35" s="14"/>
+      <c r="U35" s="14"/>
+      <c r="V35" s="14"/>
+      <c r="W35" s="14"/>
+      <c r="X35" s="14"/>
+      <c r="Y35" s="14"/>
+      <c r="Z35" s="14"/>
+    </row>
+    <row r="36" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A36" s="15"/>
+      <c r="B36" s="58"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="18" t="str">
+        <f>IFERROR(IF(OR(ISBLANK(C36),ISBLANK(D36)),"Completar",IF(D36&gt;=C36,D36-C36,"Error")),"Error")</f>
+        <v>Completar</v>
+      </c>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="21"/>
+      <c r="Q36" s="22"/>
+      <c r="R36" s="22"/>
+      <c r="S36" s="22"/>
+      <c r="T36" s="22"/>
+      <c r="U36" s="22"/>
+      <c r="V36" s="22"/>
+      <c r="W36" s="22"/>
+      <c r="X36" s="22"/>
+      <c r="Y36" s="22"/>
+      <c r="Z36" s="22"/>
+    </row>
+    <row r="37" spans="1:26" ht="6" customHeight="1">
+      <c r="A37" s="20"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="20"/>
+      <c r="P37" s="23"/>
+      <c r="Q37" s="23"/>
+      <c r="R37" s="23"/>
+      <c r="S37" s="23"/>
+      <c r="T37" s="23"/>
+      <c r="U37" s="23"/>
+      <c r="V37" s="23"/>
+      <c r="W37" s="23"/>
+      <c r="X37" s="23"/>
+      <c r="Y37" s="23"/>
+      <c r="Z37" s="23"/>
+    </row>
+    <row r="38" spans="1:26">
+      <c r="A38" s="20"/>
+      <c r="B38" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="83"/>
-      <c r="D32" s="83"/>
-      <c r="E32" s="83"/>
-      <c r="F32" s="83"/>
-      <c r="G32" s="83"/>
-      <c r="H32" s="83"/>
-      <c r="I32" s="83"/>
-      <c r="J32" s="83"/>
-      <c r="K32" s="83"/>
-      <c r="L32" s="83"/>
-      <c r="M32" s="83"/>
-      <c r="N32" s="84"/>
-      <c r="O32" s="20"/>
-      <c r="P32" s="59"/>
-      <c r="Q32" s="59"/>
-      <c r="R32" s="59"/>
-      <c r="S32" s="59"/>
-      <c r="T32" s="59"/>
-      <c r="U32" s="59"/>
-      <c r="V32" s="59"/>
-      <c r="W32" s="59"/>
-      <c r="X32" s="59"/>
-      <c r="Y32" s="59"/>
-      <c r="Z32" s="59"/>
-    </row>
-    <row r="33" spans="1:26" ht="15" customHeight="1">
-      <c r="A33" s="20"/>
-      <c r="B33" s="91" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" s="80"/>
-      <c r="D33" s="92"/>
-      <c r="E33" s="98">
-        <f>M26</f>
-        <v>85</v>
-      </c>
-      <c r="F33" s="92"/>
-      <c r="G33" s="60"/>
-      <c r="H33" s="61"/>
-      <c r="I33" s="61"/>
-      <c r="J33" s="61"/>
-      <c r="K33" s="61"/>
-      <c r="L33" s="61"/>
-      <c r="M33" s="61"/>
-      <c r="N33" s="62"/>
-      <c r="O33" s="20"/>
-      <c r="P33" s="59"/>
-      <c r="Q33" s="59"/>
-      <c r="R33" s="59"/>
-      <c r="S33" s="59"/>
-      <c r="T33" s="59"/>
-      <c r="U33" s="59"/>
-      <c r="V33" s="59"/>
-      <c r="W33" s="59"/>
-      <c r="X33" s="59"/>
-      <c r="Y33" s="59"/>
-      <c r="Z33" s="59"/>
-    </row>
-    <row r="34" spans="1:26">
-      <c r="A34" s="20"/>
-      <c r="B34" s="91" t="s">
-        <v>28</v>
-      </c>
-      <c r="C34" s="80"/>
-      <c r="D34" s="92"/>
-      <c r="E34" s="97">
-        <f>IF(M26="Completar","Completar",IFERROR(M26/(N26*24),"Error"))</f>
-        <v>83.606557377049199</v>
-      </c>
-      <c r="F34" s="92"/>
-      <c r="G34" s="63"/>
-      <c r="H34" s="64"/>
-      <c r="I34" s="64"/>
-      <c r="J34" s="64"/>
-      <c r="K34" s="64"/>
-      <c r="L34" s="64"/>
-      <c r="M34" s="64"/>
-      <c r="N34" s="65"/>
-      <c r="O34" s="20"/>
-      <c r="P34" s="59"/>
-      <c r="Q34" s="59"/>
-      <c r="R34" s="59"/>
-      <c r="S34" s="59"/>
-      <c r="T34" s="59"/>
-      <c r="U34" s="59"/>
-      <c r="V34" s="59"/>
-      <c r="W34" s="59"/>
-      <c r="X34" s="59"/>
-      <c r="Y34" s="59"/>
-      <c r="Z34" s="59"/>
-    </row>
-    <row r="35" spans="1:26" ht="15" customHeight="1">
-      <c r="A35" s="20"/>
-      <c r="B35" s="91" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35" s="80"/>
-      <c r="D35" s="92"/>
-      <c r="E35" s="98">
-        <f>IF(K26=0,0,IFERROR(ROUNDUP(K26/(M26/100),0),"Error"))</f>
-        <v>5</v>
-      </c>
-      <c r="F35" s="92"/>
-      <c r="G35" s="63"/>
-      <c r="H35" s="64"/>
-      <c r="I35" s="64"/>
-      <c r="J35" s="64"/>
-      <c r="K35" s="64"/>
-      <c r="L35" s="64"/>
-      <c r="M35" s="64"/>
-      <c r="N35" s="65"/>
-      <c r="O35" s="20"/>
-      <c r="P35" s="59"/>
-      <c r="Q35" s="59"/>
-      <c r="R35" s="59"/>
-      <c r="S35" s="59"/>
-      <c r="T35" s="59"/>
-      <c r="U35" s="59"/>
-      <c r="V35" s="59"/>
-      <c r="W35" s="59"/>
-      <c r="X35" s="59"/>
-      <c r="Y35" s="59"/>
-      <c r="Z35" s="59"/>
-    </row>
-    <row r="36" spans="1:26" ht="15" customHeight="1">
-      <c r="A36" s="20"/>
-      <c r="B36" s="91" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" s="80"/>
-      <c r="D36" s="92"/>
-      <c r="E36" s="96">
-        <f>IF(K26=0,0,IFERROR(K26/M26,"Error"))</f>
-        <v>4.7058823529411764E-2</v>
-      </c>
-      <c r="F36" s="92"/>
-      <c r="G36" s="63"/>
-      <c r="H36" s="64"/>
-      <c r="I36" s="64"/>
-      <c r="J36" s="64"/>
-      <c r="K36" s="64"/>
-      <c r="L36" s="64"/>
-      <c r="M36" s="64"/>
-      <c r="N36" s="65"/>
-      <c r="O36" s="20"/>
-      <c r="P36" s="59"/>
-      <c r="Q36" s="59"/>
-      <c r="R36" s="59"/>
-      <c r="S36" s="59"/>
-      <c r="T36" s="59"/>
-      <c r="U36" s="59"/>
-      <c r="V36" s="59"/>
-      <c r="W36" s="59"/>
-      <c r="X36" s="59"/>
-      <c r="Y36" s="59"/>
-      <c r="Z36" s="59"/>
-    </row>
-    <row r="37" spans="1:26" ht="15" customHeight="1">
-      <c r="A37" s="20"/>
-      <c r="B37" s="91" t="s">
-        <v>31</v>
-      </c>
-      <c r="C37" s="80"/>
-      <c r="D37" s="92"/>
-      <c r="E37" s="66">
-        <f>E5</f>
-        <v>6.9444444444444198E-3</v>
-      </c>
-      <c r="F37" s="67">
-        <f t="shared" ref="F37:F40" si="5">IF(E37="Completar",E37,IFERROR(E37/$E$43,"Error"))</f>
-        <v>0.1408450704225348</v>
-      </c>
-      <c r="G37" s="63"/>
-      <c r="H37" s="64"/>
-      <c r="I37" s="64"/>
-      <c r="J37" s="64"/>
-      <c r="K37" s="64"/>
-      <c r="L37" s="64"/>
-      <c r="M37" s="64"/>
-      <c r="N37" s="65"/>
-      <c r="O37" s="20"/>
-      <c r="P37" s="59"/>
-      <c r="Q37" s="59"/>
-      <c r="R37" s="59"/>
-      <c r="S37" s="59"/>
-      <c r="T37" s="59"/>
-      <c r="U37" s="59"/>
-      <c r="V37" s="59"/>
-      <c r="W37" s="59"/>
-      <c r="X37" s="59"/>
-      <c r="Y37" s="59"/>
-      <c r="Z37" s="59"/>
-    </row>
-    <row r="38" spans="1:26" ht="15" customHeight="1">
-      <c r="A38" s="20"/>
-      <c r="B38" s="91" t="s">
-        <v>32</v>
-      </c>
-      <c r="C38" s="80"/>
-      <c r="D38" s="92"/>
-      <c r="E38" s="66" t="str">
-        <f>E9</f>
-        <v>Completar</v>
-      </c>
-      <c r="F38" s="67" t="str">
-        <f t="shared" si="5"/>
-        <v>Completar</v>
-      </c>
-      <c r="G38" s="63"/>
-      <c r="H38" s="64"/>
-      <c r="I38" s="64"/>
-      <c r="J38" s="64"/>
-      <c r="K38" s="64"/>
-      <c r="L38" s="64"/>
-      <c r="M38" s="64"/>
-      <c r="N38" s="65"/>
+      <c r="C38" s="75"/>
+      <c r="D38" s="75"/>
+      <c r="E38" s="75"/>
+      <c r="F38" s="75"/>
+      <c r="G38" s="75"/>
+      <c r="H38" s="75"/>
+      <c r="I38" s="75"/>
+      <c r="J38" s="75"/>
+      <c r="K38" s="75"/>
+      <c r="L38" s="75"/>
+      <c r="M38" s="75"/>
+      <c r="N38" s="76"/>
       <c r="O38" s="20"/>
       <c r="P38" s="59"/>
       <c r="Q38" s="59"/>
@@ -2934,27 +3515,24 @@
     </row>
     <row r="39" spans="1:26" ht="15" customHeight="1">
       <c r="A39" s="20"/>
-      <c r="B39" s="91" t="s">
-        <v>33</v>
+      <c r="B39" s="80" t="s">
+        <v>27</v>
       </c>
-      <c r="C39" s="80"/>
-      <c r="D39" s="92"/>
-      <c r="E39" s="66" t="str">
-        <f>E13</f>
-        <v>Completar</v>
+      <c r="C39" s="81"/>
+      <c r="D39" s="82"/>
+      <c r="E39" s="90">
+        <f>M32</f>
+        <v>175</v>
       </c>
-      <c r="F39" s="67" t="str">
-        <f t="shared" si="5"/>
-        <v>Completar</v>
-      </c>
-      <c r="G39" s="63"/>
-      <c r="H39" s="64"/>
-      <c r="I39" s="64"/>
-      <c r="J39" s="64"/>
-      <c r="K39" s="64"/>
-      <c r="L39" s="64"/>
-      <c r="M39" s="64"/>
-      <c r="N39" s="65"/>
+      <c r="F39" s="82"/>
+      <c r="G39" s="60"/>
+      <c r="H39" s="61"/>
+      <c r="I39" s="61"/>
+      <c r="J39" s="61"/>
+      <c r="K39" s="61"/>
+      <c r="L39" s="61"/>
+      <c r="M39" s="61"/>
+      <c r="N39" s="62"/>
       <c r="O39" s="20"/>
       <c r="P39" s="59"/>
       <c r="Q39" s="59"/>
@@ -2968,21 +3546,18 @@
       <c r="Y39" s="59"/>
       <c r="Z39" s="59"/>
     </row>
-    <row r="40" spans="1:26" ht="15" customHeight="1">
+    <row r="40" spans="1:26">
       <c r="A40" s="20"/>
-      <c r="B40" s="91" t="s">
-        <v>34</v>
+      <c r="B40" s="80" t="s">
+        <v>28</v>
       </c>
-      <c r="C40" s="80"/>
-      <c r="D40" s="92"/>
-      <c r="E40" s="66" t="str">
-        <f>E30</f>
-        <v>Completar</v>
+      <c r="C40" s="81"/>
+      <c r="D40" s="82"/>
+      <c r="E40" s="89">
+        <f>IF(M32="Completar","Completar",IFERROR(M32/(N32*24),"Error"))</f>
+        <v>61.403508771929786</v>
       </c>
-      <c r="F40" s="67" t="str">
-        <f t="shared" si="5"/>
-        <v>Completar</v>
-      </c>
+      <c r="F40" s="82"/>
       <c r="G40" s="63"/>
       <c r="H40" s="64"/>
       <c r="I40" s="64"/>
@@ -3006,19 +3581,16 @@
     </row>
     <row r="41" spans="1:26" ht="15" customHeight="1">
       <c r="A41" s="20"/>
-      <c r="B41" s="91" t="s">
-        <v>35</v>
+      <c r="B41" s="80" t="s">
+        <v>29</v>
       </c>
-      <c r="C41" s="80"/>
-      <c r="D41" s="92"/>
-      <c r="E41" s="66">
-        <f>L26</f>
-        <v>7.6388888888888886E-3</v>
+      <c r="C41" s="81"/>
+      <c r="D41" s="82"/>
+      <c r="E41" s="90">
+        <f>IF(K32=0,0,IFERROR(ROUNDUP(K32/(M32/100),0),"Error"))</f>
+        <v>5</v>
       </c>
-      <c r="F41" s="67">
-        <f t="shared" ref="F41:F42" si="6">IF(E41="Completar",E41,IFERROR(E41/$E$43,"Completar"))</f>
-        <v>0.15492957746478883</v>
-      </c>
+      <c r="F41" s="82"/>
       <c r="G41" s="63"/>
       <c r="H41" s="64"/>
       <c r="I41" s="64"/>
@@ -3042,19 +3614,16 @@
     </row>
     <row r="42" spans="1:26" ht="15" customHeight="1">
       <c r="A42" s="20"/>
-      <c r="B42" s="91" t="s">
-        <v>36</v>
+      <c r="B42" s="80" t="s">
+        <v>30</v>
       </c>
-      <c r="C42" s="80"/>
-      <c r="D42" s="92"/>
-      <c r="E42" s="66">
-        <f>J26</f>
-        <v>3.472222222222221E-2</v>
+      <c r="C42" s="81"/>
+      <c r="D42" s="82"/>
+      <c r="E42" s="88">
+        <f>IF(K32=0,0,IFERROR(K32/M32,"Error"))</f>
+        <v>4.5714285714285714E-2</v>
       </c>
-      <c r="F42" s="67">
-        <f t="shared" si="6"/>
-        <v>0.70422535211267634</v>
-      </c>
+      <c r="F42" s="82"/>
       <c r="G42" s="63"/>
       <c r="H42" s="64"/>
       <c r="I42" s="64"/>
@@ -3078,24 +3647,27 @@
     </row>
     <row r="43" spans="1:26" ht="15" customHeight="1">
       <c r="A43" s="20"/>
-      <c r="B43" s="95" t="s">
-        <v>37</v>
+      <c r="B43" s="80" t="s">
+        <v>31</v>
       </c>
-      <c r="C43" s="86"/>
-      <c r="D43" s="94"/>
-      <c r="E43" s="93">
-        <f>IF(COUNTIF(E37:E42,"Error")&gt;0,"Error",IF(SUM(E37:E42)=0,"Completar",SUM(E37:E42)))</f>
-        <v>4.9305555555555519E-2</v>
+      <c r="C43" s="81"/>
+      <c r="D43" s="82"/>
+      <c r="E43" s="66">
+        <f>E5</f>
+        <v>6.9444444444444198E-3</v>
       </c>
-      <c r="F43" s="94"/>
-      <c r="G43" s="68"/>
-      <c r="H43" s="69"/>
-      <c r="I43" s="69"/>
-      <c r="J43" s="69"/>
-      <c r="K43" s="69"/>
-      <c r="L43" s="69"/>
-      <c r="M43" s="69"/>
-      <c r="N43" s="70"/>
+      <c r="F43" s="67">
+        <f t="shared" ref="F43:F46" si="3">IF(E43="Completar",E43,IFERROR(E43/$E$49,"Error"))</f>
+        <v>5.5248618784530169E-2</v>
+      </c>
+      <c r="G43" s="63"/>
+      <c r="H43" s="64"/>
+      <c r="I43" s="64"/>
+      <c r="J43" s="64"/>
+      <c r="K43" s="64"/>
+      <c r="L43" s="64"/>
+      <c r="M43" s="64"/>
+      <c r="N43" s="65"/>
       <c r="O43" s="20"/>
       <c r="P43" s="59"/>
       <c r="Q43" s="59"/>
@@ -3109,49 +3681,65 @@
       <c r="Y43" s="59"/>
       <c r="Z43" s="59"/>
     </row>
-    <row r="44" spans="1:26" ht="6" customHeight="1">
+    <row r="44" spans="1:26" ht="15" customHeight="1">
       <c r="A44" s="20"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
-      <c r="L44" s="20"/>
-      <c r="M44" s="20"/>
-      <c r="N44" s="20"/>
+      <c r="B44" s="80" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44" s="81"/>
+      <c r="D44" s="82"/>
+      <c r="E44" s="66" t="str">
+        <f>E9</f>
+        <v>Completar</v>
+      </c>
+      <c r="F44" s="67" t="str">
+        <f t="shared" si="3"/>
+        <v>Completar</v>
+      </c>
+      <c r="G44" s="63"/>
+      <c r="H44" s="64"/>
+      <c r="I44" s="64"/>
+      <c r="J44" s="64"/>
+      <c r="K44" s="64"/>
+      <c r="L44" s="64"/>
+      <c r="M44" s="64"/>
+      <c r="N44" s="65"/>
       <c r="O44" s="20"/>
-      <c r="P44" s="20"/>
-      <c r="Q44" s="20"/>
-      <c r="R44" s="20"/>
-      <c r="S44" s="20"/>
-      <c r="T44" s="20"/>
-      <c r="U44" s="20"/>
-      <c r="V44" s="20"/>
-      <c r="W44" s="20"/>
-      <c r="X44" s="20"/>
-      <c r="Y44" s="20"/>
-      <c r="Z44" s="20"/>
-    </row>
-    <row r="45" spans="1:26" hidden="1">
+      <c r="P44" s="59"/>
+      <c r="Q44" s="59"/>
+      <c r="R44" s="59"/>
+      <c r="S44" s="59"/>
+      <c r="T44" s="59"/>
+      <c r="U44" s="59"/>
+      <c r="V44" s="59"/>
+      <c r="W44" s="59"/>
+      <c r="X44" s="59"/>
+      <c r="Y44" s="59"/>
+      <c r="Z44" s="59"/>
+    </row>
+    <row r="45" spans="1:26" ht="15" customHeight="1">
       <c r="A45" s="20"/>
-      <c r="B45" s="59"/>
-      <c r="C45" s="59"/>
-      <c r="D45" s="59"/>
-      <c r="E45" s="59"/>
-      <c r="F45" s="59"/>
-      <c r="G45" s="59"/>
-      <c r="H45" s="59"/>
-      <c r="I45" s="59"/>
-      <c r="J45" s="59"/>
-      <c r="K45" s="59"/>
-      <c r="L45" s="59"/>
-      <c r="M45" s="59"/>
-      <c r="N45" s="59"/>
+      <c r="B45" s="80" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45" s="81"/>
+      <c r="D45" s="82"/>
+      <c r="E45" s="66" t="str">
+        <f>E13</f>
+        <v>Completar</v>
+      </c>
+      <c r="F45" s="67" t="str">
+        <f t="shared" si="3"/>
+        <v>Completar</v>
+      </c>
+      <c r="G45" s="63"/>
+      <c r="H45" s="64"/>
+      <c r="I45" s="64"/>
+      <c r="J45" s="64"/>
+      <c r="K45" s="64"/>
+      <c r="L45" s="64"/>
+      <c r="M45" s="64"/>
+      <c r="N45" s="65"/>
       <c r="O45" s="20"/>
       <c r="P45" s="59"/>
       <c r="Q45" s="59"/>
@@ -3165,21 +3753,29 @@
       <c r="Y45" s="59"/>
       <c r="Z45" s="59"/>
     </row>
-    <row r="46" spans="1:26">
+    <row r="46" spans="1:26" ht="15" customHeight="1">
       <c r="A46" s="20"/>
-      <c r="B46" s="59"/>
-      <c r="C46" s="59"/>
-      <c r="D46" s="59"/>
-      <c r="E46" s="59"/>
-      <c r="F46" s="59"/>
-      <c r="G46" s="59"/>
-      <c r="H46" s="59"/>
-      <c r="I46" s="59"/>
-      <c r="J46" s="59"/>
-      <c r="K46" s="59"/>
-      <c r="L46" s="59"/>
-      <c r="M46" s="59"/>
-      <c r="N46" s="59"/>
+      <c r="B46" s="80" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46" s="81"/>
+      <c r="D46" s="82"/>
+      <c r="E46" s="66" t="str">
+        <f>E36</f>
+        <v>Completar</v>
+      </c>
+      <c r="F46" s="67" t="str">
+        <f t="shared" si="3"/>
+        <v>Completar</v>
+      </c>
+      <c r="G46" s="63"/>
+      <c r="H46" s="64"/>
+      <c r="I46" s="64"/>
+      <c r="J46" s="64"/>
+      <c r="K46" s="64"/>
+      <c r="L46" s="64"/>
+      <c r="M46" s="64"/>
+      <c r="N46" s="65"/>
       <c r="O46" s="20"/>
       <c r="P46" s="59"/>
       <c r="Q46" s="59"/>
@@ -3193,21 +3789,29 @@
       <c r="Y46" s="59"/>
       <c r="Z46" s="59"/>
     </row>
-    <row r="47" spans="1:26">
+    <row r="47" spans="1:26" ht="15" customHeight="1">
       <c r="A47" s="20"/>
-      <c r="B47" s="59"/>
-      <c r="C47" s="59"/>
-      <c r="D47" s="59"/>
-      <c r="E47" s="59"/>
-      <c r="F47" s="59"/>
-      <c r="G47" s="59"/>
-      <c r="H47" s="59"/>
-      <c r="I47" s="59"/>
-      <c r="J47" s="59"/>
-      <c r="K47" s="59"/>
-      <c r="L47" s="59"/>
-      <c r="M47" s="59"/>
-      <c r="N47" s="59"/>
+      <c r="B47" s="80" t="s">
+        <v>35</v>
+      </c>
+      <c r="C47" s="81"/>
+      <c r="D47" s="82"/>
+      <c r="E47" s="66">
+        <f>L32</f>
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="F47" s="67">
+        <f t="shared" ref="F47:F48" si="4">IF(E47="Completar",E47,IFERROR(E47/$E$49,"Completar"))</f>
+        <v>0.13812154696132592</v>
+      </c>
+      <c r="G47" s="63"/>
+      <c r="H47" s="64"/>
+      <c r="I47" s="64"/>
+      <c r="J47" s="64"/>
+      <c r="K47" s="64"/>
+      <c r="L47" s="64"/>
+      <c r="M47" s="64"/>
+      <c r="N47" s="65"/>
       <c r="O47" s="20"/>
       <c r="P47" s="59"/>
       <c r="Q47" s="59"/>
@@ -3221,21 +3825,29 @@
       <c r="Y47" s="59"/>
       <c r="Z47" s="59"/>
     </row>
-    <row r="48" spans="1:26">
+    <row r="48" spans="1:26" ht="15" customHeight="1">
       <c r="A48" s="20"/>
-      <c r="B48" s="59"/>
-      <c r="C48" s="59"/>
-      <c r="D48" s="59"/>
-      <c r="E48" s="59"/>
-      <c r="F48" s="59"/>
-      <c r="G48" s="59"/>
-      <c r="H48" s="59"/>
-      <c r="I48" s="59"/>
-      <c r="J48" s="59"/>
-      <c r="K48" s="59"/>
-      <c r="L48" s="59"/>
-      <c r="M48" s="59"/>
-      <c r="N48" s="59"/>
+      <c r="B48" s="80" t="s">
+        <v>36</v>
+      </c>
+      <c r="C48" s="81"/>
+      <c r="D48" s="82"/>
+      <c r="E48" s="66">
+        <f>J32</f>
+        <v>0.10138888888888897</v>
+      </c>
+      <c r="F48" s="67">
+        <f t="shared" si="4"/>
+        <v>0.80662983425414392</v>
+      </c>
+      <c r="G48" s="63"/>
+      <c r="H48" s="64"/>
+      <c r="I48" s="64"/>
+      <c r="J48" s="64"/>
+      <c r="K48" s="64"/>
+      <c r="L48" s="64"/>
+      <c r="M48" s="64"/>
+      <c r="N48" s="65"/>
       <c r="O48" s="20"/>
       <c r="P48" s="59"/>
       <c r="Q48" s="59"/>
@@ -3249,21 +3861,26 @@
       <c r="Y48" s="59"/>
       <c r="Z48" s="59"/>
     </row>
-    <row r="49" spans="1:26">
+    <row r="49" spans="1:26" ht="15" customHeight="1">
       <c r="A49" s="20"/>
-      <c r="B49" s="59"/>
-      <c r="C49" s="59"/>
-      <c r="D49" s="59"/>
-      <c r="E49" s="59"/>
-      <c r="F49" s="59"/>
-      <c r="G49" s="59"/>
-      <c r="H49" s="59"/>
-      <c r="I49" s="59"/>
-      <c r="J49" s="59"/>
-      <c r="K49" s="59"/>
-      <c r="L49" s="59"/>
-      <c r="M49" s="59"/>
-      <c r="N49" s="59"/>
+      <c r="B49" s="85" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" s="86"/>
+      <c r="D49" s="84"/>
+      <c r="E49" s="83">
+        <f>IF(COUNTIF(E43:E48,"Error")&gt;0,"Error",IF(SUM(E43:E48)=0,"Completar",SUM(E43:E48)))</f>
+        <v>0.1256944444444445</v>
+      </c>
+      <c r="F49" s="84"/>
+      <c r="G49" s="68"/>
+      <c r="H49" s="69"/>
+      <c r="I49" s="69"/>
+      <c r="J49" s="69"/>
+      <c r="K49" s="69"/>
+      <c r="L49" s="69"/>
+      <c r="M49" s="69"/>
+      <c r="N49" s="70"/>
       <c r="O49" s="20"/>
       <c r="P49" s="59"/>
       <c r="Q49" s="59"/>
@@ -3277,35 +3894,35 @@
       <c r="Y49" s="59"/>
       <c r="Z49" s="59"/>
     </row>
-    <row r="50" spans="1:26">
+    <row r="50" spans="1:26" ht="6" customHeight="1">
       <c r="A50" s="20"/>
-      <c r="B50" s="59"/>
-      <c r="C50" s="59"/>
-      <c r="D50" s="59"/>
-      <c r="E50" s="59"/>
-      <c r="F50" s="59"/>
-      <c r="G50" s="59"/>
-      <c r="H50" s="59"/>
-      <c r="I50" s="59"/>
-      <c r="J50" s="59"/>
-      <c r="K50" s="59"/>
-      <c r="L50" s="59"/>
-      <c r="M50" s="59"/>
-      <c r="N50" s="59"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="20"/>
+      <c r="L50" s="20"/>
+      <c r="M50" s="20"/>
+      <c r="N50" s="20"/>
       <c r="O50" s="20"/>
-      <c r="P50" s="59"/>
-      <c r="Q50" s="59"/>
-      <c r="R50" s="59"/>
-      <c r="S50" s="59"/>
-      <c r="T50" s="59"/>
-      <c r="U50" s="59"/>
-      <c r="V50" s="59"/>
-      <c r="W50" s="59"/>
-      <c r="X50" s="59"/>
-      <c r="Y50" s="59"/>
-      <c r="Z50" s="59"/>
-    </row>
-    <row r="51" spans="1:26">
+      <c r="P50" s="20"/>
+      <c r="Q50" s="20"/>
+      <c r="R50" s="20"/>
+      <c r="S50" s="20"/>
+      <c r="T50" s="20"/>
+      <c r="U50" s="20"/>
+      <c r="V50" s="20"/>
+      <c r="W50" s="20"/>
+      <c r="X50" s="20"/>
+      <c r="Y50" s="20"/>
+      <c r="Z50" s="20"/>
+    </row>
+    <row r="51" spans="1:26" hidden="1">
       <c r="A51" s="20"/>
       <c r="B51" s="59"/>
       <c r="C51" s="59"/>
@@ -29905,8 +30522,219 @@
       <c r="Y1000" s="59"/>
       <c r="Z1000" s="59"/>
     </row>
+    <row r="1001" spans="1:26">
+      <c r="A1001" s="20"/>
+      <c r="B1001" s="59"/>
+      <c r="C1001" s="59"/>
+      <c r="D1001" s="59"/>
+      <c r="E1001" s="59"/>
+      <c r="F1001" s="59"/>
+      <c r="G1001" s="59"/>
+      <c r="H1001" s="59"/>
+      <c r="I1001" s="59"/>
+      <c r="J1001" s="59"/>
+      <c r="K1001" s="59"/>
+      <c r="L1001" s="59"/>
+      <c r="M1001" s="59"/>
+      <c r="N1001" s="59"/>
+      <c r="O1001" s="20"/>
+      <c r="P1001" s="59"/>
+      <c r="Q1001" s="59"/>
+      <c r="R1001" s="59"/>
+      <c r="S1001" s="59"/>
+      <c r="T1001" s="59"/>
+      <c r="U1001" s="59"/>
+      <c r="V1001" s="59"/>
+      <c r="W1001" s="59"/>
+      <c r="X1001" s="59"/>
+      <c r="Y1001" s="59"/>
+      <c r="Z1001" s="59"/>
+    </row>
+    <row r="1002" spans="1:26">
+      <c r="A1002" s="20"/>
+      <c r="B1002" s="59"/>
+      <c r="C1002" s="59"/>
+      <c r="D1002" s="59"/>
+      <c r="E1002" s="59"/>
+      <c r="F1002" s="59"/>
+      <c r="G1002" s="59"/>
+      <c r="H1002" s="59"/>
+      <c r="I1002" s="59"/>
+      <c r="J1002" s="59"/>
+      <c r="K1002" s="59"/>
+      <c r="L1002" s="59"/>
+      <c r="M1002" s="59"/>
+      <c r="N1002" s="59"/>
+      <c r="O1002" s="20"/>
+      <c r="P1002" s="59"/>
+      <c r="Q1002" s="59"/>
+      <c r="R1002" s="59"/>
+      <c r="S1002" s="59"/>
+      <c r="T1002" s="59"/>
+      <c r="U1002" s="59"/>
+      <c r="V1002" s="59"/>
+      <c r="W1002" s="59"/>
+      <c r="X1002" s="59"/>
+      <c r="Y1002" s="59"/>
+      <c r="Z1002" s="59"/>
+    </row>
+    <row r="1003" spans="1:26">
+      <c r="A1003" s="20"/>
+      <c r="B1003" s="59"/>
+      <c r="C1003" s="59"/>
+      <c r="D1003" s="59"/>
+      <c r="E1003" s="59"/>
+      <c r="F1003" s="59"/>
+      <c r="G1003" s="59"/>
+      <c r="H1003" s="59"/>
+      <c r="I1003" s="59"/>
+      <c r="J1003" s="59"/>
+      <c r="K1003" s="59"/>
+      <c r="L1003" s="59"/>
+      <c r="M1003" s="59"/>
+      <c r="N1003" s="59"/>
+      <c r="O1003" s="20"/>
+      <c r="P1003" s="59"/>
+      <c r="Q1003" s="59"/>
+      <c r="R1003" s="59"/>
+      <c r="S1003" s="59"/>
+      <c r="T1003" s="59"/>
+      <c r="U1003" s="59"/>
+      <c r="V1003" s="59"/>
+      <c r="W1003" s="59"/>
+      <c r="X1003" s="59"/>
+      <c r="Y1003" s="59"/>
+      <c r="Z1003" s="59"/>
+    </row>
+    <row r="1004" spans="1:26">
+      <c r="A1004" s="20"/>
+      <c r="B1004" s="59"/>
+      <c r="C1004" s="59"/>
+      <c r="D1004" s="59"/>
+      <c r="E1004" s="59"/>
+      <c r="F1004" s="59"/>
+      <c r="G1004" s="59"/>
+      <c r="H1004" s="59"/>
+      <c r="I1004" s="59"/>
+      <c r="J1004" s="59"/>
+      <c r="K1004" s="59"/>
+      <c r="L1004" s="59"/>
+      <c r="M1004" s="59"/>
+      <c r="N1004" s="59"/>
+      <c r="O1004" s="20"/>
+      <c r="P1004" s="59"/>
+      <c r="Q1004" s="59"/>
+      <c r="R1004" s="59"/>
+      <c r="S1004" s="59"/>
+      <c r="T1004" s="59"/>
+      <c r="U1004" s="59"/>
+      <c r="V1004" s="59"/>
+      <c r="W1004" s="59"/>
+      <c r="X1004" s="59"/>
+      <c r="Y1004" s="59"/>
+      <c r="Z1004" s="59"/>
+    </row>
+    <row r="1005" spans="1:26">
+      <c r="A1005" s="20"/>
+      <c r="B1005" s="59"/>
+      <c r="C1005" s="59"/>
+      <c r="D1005" s="59"/>
+      <c r="E1005" s="59"/>
+      <c r="F1005" s="59"/>
+      <c r="G1005" s="59"/>
+      <c r="H1005" s="59"/>
+      <c r="I1005" s="59"/>
+      <c r="J1005" s="59"/>
+      <c r="K1005" s="59"/>
+      <c r="L1005" s="59"/>
+      <c r="M1005" s="59"/>
+      <c r="N1005" s="59"/>
+      <c r="O1005" s="20"/>
+      <c r="P1005" s="59"/>
+      <c r="Q1005" s="59"/>
+      <c r="R1005" s="59"/>
+      <c r="S1005" s="59"/>
+      <c r="T1005" s="59"/>
+      <c r="U1005" s="59"/>
+      <c r="V1005" s="59"/>
+      <c r="W1005" s="59"/>
+      <c r="X1005" s="59"/>
+      <c r="Y1005" s="59"/>
+      <c r="Z1005" s="59"/>
+    </row>
+    <row r="1006" spans="1:26">
+      <c r="A1006" s="20"/>
+      <c r="B1006" s="59"/>
+      <c r="C1006" s="59"/>
+      <c r="D1006" s="59"/>
+      <c r="E1006" s="59"/>
+      <c r="F1006" s="59"/>
+      <c r="G1006" s="59"/>
+      <c r="H1006" s="59"/>
+      <c r="I1006" s="59"/>
+      <c r="J1006" s="59"/>
+      <c r="K1006" s="59"/>
+      <c r="L1006" s="59"/>
+      <c r="M1006" s="59"/>
+      <c r="N1006" s="59"/>
+      <c r="O1006" s="20"/>
+      <c r="P1006" s="59"/>
+      <c r="Q1006" s="59"/>
+      <c r="R1006" s="59"/>
+      <c r="S1006" s="59"/>
+      <c r="T1006" s="59"/>
+      <c r="U1006" s="59"/>
+      <c r="V1006" s="59"/>
+      <c r="W1006" s="59"/>
+      <c r="X1006" s="59"/>
+      <c r="Y1006" s="59"/>
+      <c r="Z1006" s="59"/>
+    </row>
   </sheetData>
-  <mergeCells count="44">
+  <mergeCells count="50">
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B38:N38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B15:N15"/>
+    <mergeCell ref="F12:N12"/>
+    <mergeCell ref="F13:N13"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="E40:F40"/>
     <mergeCell ref="D1:N1"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B7:E7"/>
@@ -29914,55 +30742,79 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="F8:N8"/>
     <mergeCell ref="F9:N9"/>
-    <mergeCell ref="B15:N15"/>
-    <mergeCell ref="F12:N12"/>
-    <mergeCell ref="F13:N13"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B32:N32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:B1048576 D1:XFD1048576 C3:C1048576">
+  <conditionalFormatting sqref="D1:XFD24 C3:C24 A32:XFD1048576 N25:XFD31 A1:B31">
+    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
+      <formula>"Completar"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:XFD24 C3:C24 A32:XFD1048576 N25:XFD31 A1:B31">
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
+      <formula>"Error"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25:M25 C26:E26">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
+      <formula>"Completar"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25:M25 C26:E26">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+      <formula>"Error"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31:I31 F26:M26 K31:M31 J27:J31">
+    <cfRule type="cellIs" dxfId="21" priority="17" operator="equal">
+      <formula>"Completar"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31:I31 F26:M26 K31:M31 J27:J31">
+    <cfRule type="cellIs" dxfId="20" priority="18" operator="equal">
+      <formula>"Error"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27:I27 K27:M27">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+      <formula>"Completar"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27:I27 K27:M27">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+      <formula>"Error"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28:I28 K28:M28">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"Completar"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28:I28 K28:M28">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"Error"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29:I29 K29:M29">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"Completar"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29:I29 K29:M29">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"Error"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30:I30 K30:M30">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:B1048576 D1:XFD1048576 C3:C1048576">
+  <conditionalFormatting sqref="C30:I30 K30:M30">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>